<commit_message>
image donee weeee - done by prabhas
</commit_message>
<xml_diff>
--- a/databases/activity_log.xlsx
+++ b/databases/activity_log.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D151"/>
+  <dimension ref="A1:D164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3751,6 +3751,292 @@
         </is>
       </c>
     </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>09:40:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>09:41:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>09:42:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>09:48:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>09:55:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>09:57:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>09:58:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>10:00:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>10:09:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>10:17:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>10:19:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>10:28:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>10:29:17</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
login page left,else done
</commit_message>
<xml_diff>
--- a/databases/activity_log.xlsx
+++ b/databases/activity_log.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D197"/>
+  <dimension ref="A1:D201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4763,6 +4763,94 @@
         </is>
       </c>
     </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>11:40:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>11:41:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>11:43:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>LOG-OUT</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>11:43:46</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
view items, filters done
</commit_message>
<xml_diff>
--- a/databases/activity_log.xlsx
+++ b/databases/activity_log.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D201"/>
+  <dimension ref="A1:D213"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4851,6 +4851,271 @@
         </is>
       </c>
     </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>12:48:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Added item barcode no: 6454</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>13:39:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Item checked out to FSL barcode no: 6454</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>13:40:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Item checked in from FSL barcode no: 6454</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>13:40:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>LOG-OUT</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>13:48:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>21:56:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>22:01:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>22:02:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>22:05:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Item checked out to FSL barcode no: 1003</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>22:07:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Item checked in from FSL barcode no: 1003</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>22:07:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>02/09/24</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>22:12:27</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
log me green line h aur print baaki h
</commit_message>
<xml_diff>
--- a/databases/activity_log.xlsx
+++ b/databases/activity_log.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D353"/>
+  <dimension ref="A1:D386"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8196,6 +8196,732 @@
         </is>
       </c>
     </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>05/13/24</t>
+        </is>
+      </c>
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>14:58:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>05/13/24</t>
+        </is>
+      </c>
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>14:59:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>05/13/24</t>
+        </is>
+      </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>15:04:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>05/13/24</t>
+        </is>
+      </c>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>16:11:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>05/13/24</t>
+        </is>
+      </c>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>16:11:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>05/13/24</t>
+        </is>
+      </c>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>16:11:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>05/13/24</t>
+        </is>
+      </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>16:12:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>05/13/24</t>
+        </is>
+      </c>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>16:13:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>05/13/24</t>
+        </is>
+      </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>16:14:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>14:17:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>14:18:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>14:35:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>14:36:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>14:43:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>14:51:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D369" t="inlineStr">
+        <is>
+          <t>15:43:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D370" t="inlineStr">
+        <is>
+          <t>15:49:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D371" t="inlineStr">
+        <is>
+          <t>21:29:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D372" t="inlineStr">
+        <is>
+          <t>21:33:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D373" t="inlineStr">
+        <is>
+          <t>21:41:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D374" t="inlineStr">
+        <is>
+          <t>21:46:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D375" t="inlineStr">
+        <is>
+          <t>21:47:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>21:51:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>21:54:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D378" t="inlineStr">
+        <is>
+          <t>21:55:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>22:00:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>22:00:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>22:07:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>22:08:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>22:08:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>22:24:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>22:24:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>LOG-IN</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>05/14/24</t>
+        </is>
+      </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>22:25:22</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>